<commit_message>
Cambio en la variables de fecha por Unidad, se trabajan tipo Date y luego una Date con formato para poder visualizar en consola
</commit_message>
<xml_diff>
--- a/SOF-S-MA-3-2-signed-3-8.xlsx
+++ b/SOF-S-MA-3-2-signed-3-8.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\NetBeansProjects\testExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Desktop\Proyecto Ecturas de datos\testExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B51495A-B6E5-4DB8-81A7-6008D400DF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53679DF2-DCCE-4153-885A-4164E55A17DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2294,7 +2294,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2403,6 +2403,12 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="5.5"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2644,7 +2650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2741,51 +2747,84 @@
     <xf numFmtId="1" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="23"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="23"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="23"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2795,14 +2834,44 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="23"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="23"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="23"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2813,27 +2882,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -2852,32 +2900,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="40"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="40"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="40"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -2933,71 +2984,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="40"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="40"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="40"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3303,10 +3318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="F3" sqref="F3:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3319,17 +3334,17 @@
     <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="52"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="38"/>
+    </row>
+    <row r="2" spans="1:8" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
@@ -3349,25 +3364,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="105" t="s">
+    <row r="3" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44">
+      <c r="D3" s="47"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="117">
         <v>45048</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
-      <c r="B4" s="39"/>
+    <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="40"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="26" t="s">
         <v>169</v>
       </c>
@@ -3377,41 +3392,41 @@
       <c r="E4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="45"/>
-    </row>
-    <row r="5" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="108" t="s">
+      <c r="F4" s="118"/>
+    </row>
+    <row r="5" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="40"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="109"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="45"/>
-    </row>
-    <row r="6" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
-      <c r="B6" s="106"/>
-      <c r="C6" s="114"/>
-      <c r="D6" s="116">
+      <c r="D5" s="52"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="118"/>
+    </row>
+    <row r="6" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="40"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="34">
         <v>0</v>
       </c>
-      <c r="E6" s="114"/>
-      <c r="F6" s="107"/>
-    </row>
-    <row r="7" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="111" t="s">
+      <c r="E6" s="32"/>
+      <c r="F6" s="119"/>
+    </row>
+    <row r="7" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="40"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="112"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="45"/>
-    </row>
-    <row r="8" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37"/>
-      <c r="B8" s="40"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="118"/>
+    </row>
+    <row r="8" spans="1:8" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="41"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="25" t="s">
         <v>12</v>
       </c>
@@ -3421,27 +3436,27 @@
       <c r="E8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="46"/>
-    </row>
-    <row r="9" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
+      <c r="F8" s="120"/>
+    </row>
+    <row r="9" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="44">
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="113">
         <v>45049</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
-      <c r="B10" s="39"/>
+    <row r="10" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="40"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="25" t="s">
         <v>15</v>
       </c>
@@ -3451,21 +3466,22 @@
       <c r="E10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="45"/>
-    </row>
-    <row r="11" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="41" t="s">
+      <c r="F10" s="114"/>
+    </row>
+    <row r="11" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="45"/>
-    </row>
-    <row r="12" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
-      <c r="B12" s="39"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="114"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="1:8" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="40"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="25" t="s">
         <v>16</v>
       </c>
@@ -3475,21 +3491,21 @@
       <c r="E12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="45"/>
-    </row>
-    <row r="13" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="41" t="s">
+      <c r="F12" s="115"/>
+    </row>
+    <row r="13" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="40"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="45"/>
-    </row>
-    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
-      <c r="B14" s="40"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="114"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="41"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="25" t="s">
         <v>18</v>
       </c>
@@ -3499,27 +3515,27 @@
       <c r="E14" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="46"/>
-    </row>
-    <row r="15" spans="1:6" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
+      <c r="F14" s="116"/>
+    </row>
+    <row r="15" spans="1:8" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="44">
+      <c r="D15" s="47"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="113">
         <v>45055</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="36"/>
-      <c r="B16" s="39"/>
+    <row r="16" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="40"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="25" t="s">
         <v>22</v>
       </c>
@@ -3529,41 +3545,41 @@
       <c r="E16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="45"/>
+      <c r="F16" s="114"/>
     </row>
     <row r="17" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="41" t="s">
+      <c r="A17" s="40"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="45"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="114"/>
     </row>
     <row r="18" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="36"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="114"/>
-      <c r="D18" s="115">
+      <c r="A18" s="40"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33">
         <v>0</v>
       </c>
-      <c r="E18" s="114"/>
-      <c r="F18" s="45"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="115"/>
     </row>
     <row r="19" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="36"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="41" t="s">
+      <c r="A19" s="40"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="45"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="114"/>
     </row>
     <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37"/>
-      <c r="B20" s="40"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="25" t="s">
         <v>23</v>
       </c>
@@ -3573,27 +3589,27 @@
       <c r="E20" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="46"/>
+      <c r="F20" s="116"/>
     </row>
     <row r="21" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="44">
+      <c r="D21" s="47"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="113">
         <v>45056</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="48"/>
-      <c r="B22" s="39"/>
+      <c r="A22" s="59"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="25" t="s">
         <v>15</v>
       </c>
@@ -3603,21 +3619,21 @@
       <c r="E22" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="45"/>
+      <c r="F22" s="114"/>
     </row>
     <row r="23" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="48"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="41" t="s">
+      <c r="A23" s="59"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="45"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="114"/>
     </row>
     <row r="24" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="48"/>
-      <c r="B24" s="39"/>
+      <c r="A24" s="59"/>
+      <c r="B24" s="43"/>
       <c r="C24" s="25" t="s">
         <v>25</v>
       </c>
@@ -3627,21 +3643,21 @@
       <c r="E24" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="45"/>
+      <c r="F24" s="115"/>
     </row>
     <row r="25" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="48"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="41" t="s">
+      <c r="A25" s="59"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="45"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="114"/>
     </row>
     <row r="26" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
-      <c r="B26" s="40"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="25" t="s">
         <v>27</v>
       </c>
@@ -3651,27 +3667,27 @@
       <c r="E26" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="46"/>
+      <c r="F26" s="116"/>
     </row>
     <row r="27" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="42"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="44">
+      <c r="D27" s="47"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="113">
         <v>45062</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="36"/>
-      <c r="B28" s="39"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="43"/>
       <c r="C28" s="25" t="s">
         <v>22</v>
       </c>
@@ -3681,41 +3697,41 @@
       <c r="E28" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="45"/>
+      <c r="F28" s="114"/>
     </row>
     <row r="29" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="36"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="41" t="s">
+      <c r="A29" s="40"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="45"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="114"/>
     </row>
     <row r="30" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="115">
+      <c r="A30" s="40"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="33">
         <v>0</v>
       </c>
-      <c r="E30" s="114"/>
-      <c r="F30" s="45"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="115"/>
     </row>
     <row r="31" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="36"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="41" t="s">
+      <c r="A31" s="40"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="45"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="114"/>
     </row>
     <row r="32" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="37"/>
-      <c r="B32" s="40"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="45"/>
       <c r="C32" s="25" t="s">
         <v>29</v>
       </c>
@@ -3725,27 +3741,27 @@
       <c r="E32" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="46"/>
+      <c r="F32" s="116"/>
     </row>
     <row r="33" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="42"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="32">
+      <c r="D33" s="47"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="113">
         <v>45063</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="48"/>
-      <c r="B34" s="39"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="43"/>
       <c r="C34" s="25" t="s">
         <v>15</v>
       </c>
@@ -3755,21 +3771,21 @@
       <c r="E34" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="33"/>
+      <c r="F34" s="114"/>
     </row>
     <row r="35" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="41" t="s">
+      <c r="A35" s="59"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="42"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="33"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="114"/>
     </row>
     <row r="36" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="48"/>
-      <c r="B36" s="39"/>
+      <c r="A36" s="59"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="25" t="s">
         <v>31</v>
       </c>
@@ -3779,21 +3795,21 @@
       <c r="E36" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F36" s="33"/>
+      <c r="F36" s="115"/>
     </row>
     <row r="37" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="48"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="41" t="s">
+      <c r="A37" s="59"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="42"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="33"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="114"/>
     </row>
     <row r="38" spans="1:6" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="49"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="60"/>
+      <c r="B38" s="45"/>
       <c r="C38" s="25" t="s">
         <v>33</v>
       </c>
@@ -3803,27 +3819,27 @@
       <c r="E38" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="34"/>
+      <c r="F38" s="116"/>
     </row>
     <row r="39" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="41" t="s">
+      <c r="C39" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="42"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="44">
+      <c r="D39" s="47"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="113">
         <v>45069</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="36"/>
-      <c r="B40" s="39"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="43"/>
       <c r="C40" s="25" t="s">
         <v>22</v>
       </c>
@@ -3833,41 +3849,41 @@
       <c r="E40" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="45"/>
+      <c r="F40" s="114"/>
     </row>
     <row r="41" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="41" t="s">
+      <c r="A41" s="40"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="42"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="45"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="114"/>
     </row>
     <row r="42" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="36"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="114"/>
-      <c r="D42" s="115">
+      <c r="A42" s="40"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="33">
         <v>0</v>
       </c>
-      <c r="E42" s="114"/>
-      <c r="F42" s="45"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="115"/>
     </row>
     <row r="43" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="36"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="41" t="s">
+      <c r="A43" s="40"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="45"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="114"/>
     </row>
     <row r="44" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="37"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="25" t="s">
         <v>35</v>
       </c>
@@ -3877,27 +3893,27 @@
       <c r="E44" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F44" s="46"/>
+      <c r="F44" s="116"/>
     </row>
     <row r="45" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="41" t="s">
+      <c r="C45" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="42"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="32">
+      <c r="D45" s="47"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="113">
         <v>45070</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="36"/>
-      <c r="B46" s="39"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="43"/>
       <c r="C46" s="25" t="s">
         <v>15</v>
       </c>
@@ -3907,21 +3923,21 @@
       <c r="E46" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F46" s="33"/>
+      <c r="F46" s="114"/>
     </row>
     <row r="47" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="36"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="41" t="s">
+      <c r="A47" s="40"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D47" s="42"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="33"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="114"/>
     </row>
     <row r="48" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="36"/>
-      <c r="B48" s="39"/>
+      <c r="A48" s="40"/>
+      <c r="B48" s="43"/>
       <c r="C48" s="25" t="s">
         <v>38</v>
       </c>
@@ -3931,21 +3947,21 @@
       <c r="E48" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F48" s="33"/>
+      <c r="F48" s="115"/>
     </row>
     <row r="49" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="36"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="41" t="s">
+      <c r="A49" s="40"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="42"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="33"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="114"/>
     </row>
     <row r="50" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="40"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="45"/>
       <c r="C50" s="25" t="s">
         <v>40</v>
       </c>
@@ -3955,47 +3971,13 @@
       <c r="E50" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F50" s="34"/>
+      <c r="F50" s="116"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D54" s="117"/>
+      <c r="D54" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:F8"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:F14"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:F20"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:F26"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C27:E27"/>
     <mergeCell ref="F33:F38"/>
     <mergeCell ref="F45:F50"/>
     <mergeCell ref="A45:A50"/>
@@ -4011,6 +3993,40 @@
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="A33:A38"/>
     <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:F26"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:F20"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:F14"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:F8"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4036,24 +4052,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62" t="s">
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="70" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="76"/>
-      <c r="B2" s="73"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
@@ -4063,39 +4079,39 @@
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="45"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="76"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="59" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="45"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="76"/>
-      <c r="B4" s="73"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="45"/>
+      <c r="F4" s="49"/>
     </row>
     <row r="5" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="76"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="59" t="s">
+      <c r="A5" s="62"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="60"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="45"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="49"/>
     </row>
     <row r="6" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="77"/>
-      <c r="B6" s="74"/>
+      <c r="A6" s="63"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="1" t="s">
         <v>42</v>
       </c>
@@ -4105,25 +4121,25 @@
       <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="46"/>
+      <c r="F6" s="50"/>
     </row>
     <row r="7" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="61"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="73"/>
-      <c r="B8" s="57"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
@@ -4133,23 +4149,23 @@
       <c r="E8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="70" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="73"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="59" t="s">
+      <c r="A9" s="65"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="45"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="49"/>
     </row>
     <row r="10" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="73"/>
-      <c r="B10" s="57"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="3" t="s">
         <v>46</v>
       </c>
@@ -4159,21 +4175,21 @@
       <c r="E10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="45"/>
+      <c r="F10" s="49"/>
     </row>
     <row r="11" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="73"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="59" t="s">
+      <c r="A11" s="65"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="45"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="49"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="74"/>
-      <c r="B12" s="58"/>
+      <c r="A12" s="66"/>
+      <c r="B12" s="73"/>
       <c r="C12" s="3" t="s">
         <v>48</v>
       </c>
@@ -4183,27 +4199,27 @@
       <c r="E12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="46"/>
+      <c r="F12" s="50"/>
     </row>
     <row r="13" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="60"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62" t="s">
+      <c r="D13" s="68"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="70" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="73"/>
-      <c r="B14" s="57"/>
+      <c r="A14" s="65"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
@@ -4213,39 +4229,39 @@
       <c r="E14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="45"/>
+      <c r="F14" s="49"/>
     </row>
     <row r="15" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="73"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="59" t="s">
+      <c r="A15" s="65"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="45"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="49"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="73"/>
-      <c r="B16" s="57"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="45"/>
+      <c r="F16" s="49"/>
     </row>
     <row r="17" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="73"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="59" t="s">
+      <c r="A17" s="65"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="45"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="49"/>
     </row>
     <row r="18" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="74"/>
-      <c r="B18" s="58"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="73"/>
       <c r="C18" s="3" t="s">
         <v>35</v>
       </c>
@@ -4255,25 +4271,25 @@
       <c r="E18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="46"/>
+      <c r="F18" s="50"/>
     </row>
     <row r="19" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="60"/>
-      <c r="E19" s="61"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="69"/>
       <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="54"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="3" t="s">
         <v>15</v>
       </c>
@@ -4283,23 +4299,23 @@
       <c r="E20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="62" t="s">
+      <c r="F20" s="70" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="54"/>
-      <c r="B21" s="73"/>
-      <c r="C21" s="59" t="s">
+      <c r="A21" s="75"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="45"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="49"/>
     </row>
     <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="54"/>
-      <c r="B22" s="73"/>
+      <c r="A22" s="75"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="1" t="s">
         <v>54</v>
       </c>
@@ -4309,21 +4325,21 @@
       <c r="E22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="45"/>
+      <c r="F22" s="49"/>
     </row>
     <row r="23" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="54"/>
-      <c r="B23" s="73"/>
-      <c r="C23" s="59" t="s">
+      <c r="A23" s="75"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="45"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="49"/>
     </row>
     <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="55"/>
-      <c r="B24" s="74"/>
+      <c r="A24" s="76"/>
+      <c r="B24" s="66"/>
       <c r="C24" s="1" t="s">
         <v>55</v>
       </c>
@@ -4333,27 +4349,27 @@
       <c r="E24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F24" s="46"/>
+      <c r="F24" s="50"/>
     </row>
     <row r="25" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="62" t="s">
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="70" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="73"/>
-      <c r="B26" s="73"/>
+      <c r="A26" s="65"/>
+      <c r="B26" s="65"/>
       <c r="C26" s="3" t="s">
         <v>22</v>
       </c>
@@ -4363,39 +4379,39 @@
       <c r="E26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="45"/>
+      <c r="F26" s="49"/>
     </row>
     <row r="27" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="73"/>
-      <c r="B27" s="73"/>
-      <c r="C27" s="59" t="s">
+      <c r="A27" s="65"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="60"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="45"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="49"/>
     </row>
     <row r="28" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="65"/>
+      <c r="B28" s="65"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="45"/>
+      <c r="F28" s="49"/>
     </row>
     <row r="29" spans="1:6" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="73"/>
-      <c r="B29" s="73"/>
-      <c r="C29" s="59" t="s">
+      <c r="A29" s="65"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="60"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="45"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="49"/>
     </row>
     <row r="30" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="74"/>
-      <c r="B30" s="74"/>
+      <c r="A30" s="66"/>
+      <c r="B30" s="66"/>
       <c r="C30" s="3" t="s">
         <v>35</v>
       </c>
@@ -4405,25 +4421,25 @@
       <c r="E30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="46"/>
+      <c r="F30" s="50"/>
     </row>
     <row r="31" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="72" t="s">
+      <c r="A31" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="72" t="s">
+      <c r="B31" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="59" t="s">
+      <c r="C31" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="60"/>
-      <c r="E31" s="61"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="69"/>
       <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="73"/>
-      <c r="B32" s="73"/>
+      <c r="A32" s="65"/>
+      <c r="B32" s="65"/>
       <c r="C32" s="3" t="s">
         <v>15</v>
       </c>
@@ -4433,23 +4449,23 @@
       <c r="E32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="62" t="s">
+      <c r="F32" s="70" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="73"/>
-      <c r="B33" s="73"/>
-      <c r="C33" s="59" t="s">
+      <c r="A33" s="65"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="60"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="45"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="49"/>
     </row>
     <row r="34" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="73"/>
-      <c r="B34" s="73"/>
+      <c r="A34" s="65"/>
+      <c r="B34" s="65"/>
       <c r="C34" s="3" t="s">
         <v>60</v>
       </c>
@@ -4459,21 +4475,21 @@
       <c r="E34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F34" s="45"/>
+      <c r="F34" s="49"/>
     </row>
     <row r="35" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="73"/>
-      <c r="B35" s="73"/>
-      <c r="C35" s="59" t="s">
+      <c r="A35" s="65"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="60"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="45"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="49"/>
     </row>
     <row r="36" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="74"/>
-      <c r="B36" s="74"/>
+      <c r="A36" s="66"/>
+      <c r="B36" s="66"/>
       <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
@@ -4483,27 +4499,27 @@
       <c r="E36" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="46"/>
+      <c r="F36" s="50"/>
     </row>
     <row r="37" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="53" t="s">
+      <c r="A37" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="72" t="s">
+      <c r="B37" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="59" t="s">
+      <c r="C37" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="60"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="62" t="s">
+      <c r="D37" s="68"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="70" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="54"/>
-      <c r="B38" s="73"/>
+      <c r="A38" s="75"/>
+      <c r="B38" s="65"/>
       <c r="C38" s="3" t="s">
         <v>22</v>
       </c>
@@ -4513,39 +4529,39 @@
       <c r="E38" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="45"/>
+      <c r="F38" s="49"/>
     </row>
     <row r="39" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="54"/>
-      <c r="B39" s="73"/>
-      <c r="C39" s="59" t="s">
+      <c r="A39" s="75"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="60"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="45"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="49"/>
     </row>
     <row r="40" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="54"/>
-      <c r="B40" s="73"/>
+      <c r="A40" s="75"/>
+      <c r="B40" s="65"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="45"/>
+      <c r="F40" s="49"/>
     </row>
     <row r="41" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="54"/>
-      <c r="B41" s="73"/>
-      <c r="C41" s="59" t="s">
+      <c r="A41" s="75"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="60"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="45"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="49"/>
     </row>
     <row r="42" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="55"/>
-      <c r="B42" s="74"/>
+      <c r="A42" s="76"/>
+      <c r="B42" s="66"/>
       <c r="C42" s="3" t="s">
         <v>35</v>
       </c>
@@ -4555,25 +4571,25 @@
       <c r="E42" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F42" s="46"/>
+      <c r="F42" s="50"/>
     </row>
     <row r="43" spans="1:6" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="59" t="s">
+      <c r="C43" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="60"/>
-      <c r="E43" s="61"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="69"/>
       <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="54"/>
-      <c r="B44" s="57"/>
+      <c r="A44" s="75"/>
+      <c r="B44" s="72"/>
       <c r="C44" s="3" t="s">
         <v>15</v>
       </c>
@@ -4583,23 +4599,23 @@
       <c r="E44" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F44" s="62" t="s">
+      <c r="F44" s="70" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="54"/>
-      <c r="B45" s="57"/>
-      <c r="C45" s="59" t="s">
+      <c r="A45" s="75"/>
+      <c r="B45" s="72"/>
+      <c r="C45" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D45" s="60"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="45"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="49"/>
     </row>
     <row r="46" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="54"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="75"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="1" t="s">
         <v>67</v>
       </c>
@@ -4609,21 +4625,21 @@
       <c r="E46" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F46" s="45"/>
+      <c r="F46" s="49"/>
     </row>
     <row r="47" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="54"/>
-      <c r="B47" s="57"/>
-      <c r="C47" s="59" t="s">
+      <c r="A47" s="75"/>
+      <c r="B47" s="72"/>
+      <c r="C47" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="60"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="45"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="49"/>
     </row>
     <row r="48" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="55"/>
-      <c r="B48" s="58"/>
+      <c r="A48" s="76"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="3" t="s">
         <v>69</v>
       </c>
@@ -4633,27 +4649,27 @@
       <c r="E48" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F48" s="46"/>
+      <c r="F48" s="50"/>
     </row>
     <row r="49" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="63" t="s">
+      <c r="A49" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="66" t="s">
+      <c r="B49" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="59" t="s">
+      <c r="C49" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="60"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="62" t="s">
+      <c r="D49" s="68"/>
+      <c r="E49" s="69"/>
+      <c r="F49" s="70" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="64"/>
-      <c r="B50" s="67"/>
+      <c r="A50" s="78"/>
+      <c r="B50" s="81"/>
       <c r="C50" s="3" t="s">
         <v>74</v>
       </c>
@@ -4663,39 +4679,39 @@
       <c r="E50" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F50" s="45"/>
+      <c r="F50" s="49"/>
     </row>
     <row r="51" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="64"/>
-      <c r="B51" s="67"/>
-      <c r="C51" s="59" t="s">
+      <c r="A51" s="78"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="60"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="45"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="49"/>
     </row>
     <row r="52" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="64"/>
-      <c r="B52" s="67"/>
+      <c r="A52" s="78"/>
+      <c r="B52" s="81"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
-      <c r="F52" s="45"/>
+      <c r="F52" s="49"/>
     </row>
     <row r="53" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="64"/>
-      <c r="B53" s="67"/>
-      <c r="C53" s="59" t="s">
+      <c r="A53" s="78"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D53" s="60"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="45"/>
+      <c r="D53" s="68"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="49"/>
     </row>
     <row r="54" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="65"/>
-      <c r="B54" s="68"/>
+      <c r="A54" s="79"/>
+      <c r="B54" s="82"/>
       <c r="C54" s="1" t="s">
         <v>76</v>
       </c>
@@ -4705,23 +4721,23 @@
       <c r="E54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F54" s="46"/>
+      <c r="F54" s="50"/>
     </row>
     <row r="55" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11"/>
       <c r="B55" s="11"/>
-      <c r="C55" s="59" t="s">
+      <c r="C55" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="60"/>
-      <c r="E55" s="61"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="69"/>
       <c r="F55" s="12"/>
     </row>
     <row r="56" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="54" t="s">
+      <c r="A56" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="B56" s="70" t="s">
+      <c r="B56" s="83" t="s">
         <v>78</v>
       </c>
       <c r="C56" s="10" t="s">
@@ -4733,23 +4749,23 @@
       <c r="E56" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F56" s="62" t="s">
+      <c r="F56" s="70" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="54"/>
-      <c r="B57" s="70"/>
-      <c r="C57" s="59" t="s">
+      <c r="A57" s="75"/>
+      <c r="B57" s="83"/>
+      <c r="C57" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D57" s="60"/>
-      <c r="E57" s="61"/>
-      <c r="F57" s="45"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="69"/>
+      <c r="F57" s="49"/>
     </row>
     <row r="58" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="54"/>
-      <c r="B58" s="70"/>
+      <c r="A58" s="75"/>
+      <c r="B58" s="83"/>
       <c r="C58" s="1" t="s">
         <v>80</v>
       </c>
@@ -4759,21 +4775,21 @@
       <c r="E58" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F58" s="45"/>
+      <c r="F58" s="49"/>
     </row>
     <row r="59" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="54"/>
-      <c r="B59" s="70"/>
-      <c r="C59" s="59" t="s">
+      <c r="A59" s="75"/>
+      <c r="B59" s="83"/>
+      <c r="C59" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="60"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="45"/>
+      <c r="D59" s="68"/>
+      <c r="E59" s="69"/>
+      <c r="F59" s="49"/>
     </row>
     <row r="60" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="55"/>
-      <c r="B60" s="71"/>
+      <c r="A60" s="76"/>
+      <c r="B60" s="84"/>
       <c r="C60" s="1" t="s">
         <v>27</v>
       </c>
@@ -4783,27 +4799,27 @@
       <c r="E60" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F60" s="46"/>
+      <c r="F60" s="50"/>
     </row>
     <row r="61" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="53" t="s">
+      <c r="A61" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="B61" s="56" t="s">
+      <c r="B61" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="C61" s="59" t="s">
+      <c r="C61" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="60"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="62" t="s">
+      <c r="D61" s="68"/>
+      <c r="E61" s="69"/>
+      <c r="F61" s="70" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="54"/>
-      <c r="B62" s="57"/>
+      <c r="A62" s="75"/>
+      <c r="B62" s="72"/>
       <c r="C62" s="3" t="s">
         <v>22</v>
       </c>
@@ -4813,39 +4829,39 @@
       <c r="E62" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F62" s="45"/>
+      <c r="F62" s="49"/>
     </row>
     <row r="63" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="54"/>
-      <c r="B63" s="57"/>
-      <c r="C63" s="59" t="s">
+      <c r="A63" s="75"/>
+      <c r="B63" s="72"/>
+      <c r="C63" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="60"/>
-      <c r="E63" s="61"/>
-      <c r="F63" s="45"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="69"/>
+      <c r="F63" s="49"/>
     </row>
     <row r="64" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="54"/>
-      <c r="B64" s="57"/>
+      <c r="A64" s="75"/>
+      <c r="B64" s="72"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
-      <c r="F64" s="45"/>
+      <c r="F64" s="49"/>
     </row>
     <row r="65" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="54"/>
-      <c r="B65" s="57"/>
-      <c r="C65" s="59" t="s">
+      <c r="A65" s="75"/>
+      <c r="B65" s="72"/>
+      <c r="C65" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D65" s="60"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="45"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="69"/>
+      <c r="F65" s="49"/>
     </row>
     <row r="66" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="55"/>
-      <c r="B66" s="58"/>
+      <c r="A66" s="76"/>
+      <c r="B66" s="73"/>
       <c r="C66" s="3" t="s">
         <v>83</v>
       </c>
@@ -4855,25 +4871,25 @@
       <c r="E66" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F66" s="46"/>
+      <c r="F66" s="50"/>
     </row>
     <row r="67" spans="1:6" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="53" t="s">
+      <c r="A67" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="B67" s="69" t="s">
+      <c r="B67" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="C67" s="59" t="s">
+      <c r="C67" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D67" s="60"/>
-      <c r="E67" s="61"/>
+      <c r="D67" s="68"/>
+      <c r="E67" s="69"/>
       <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="54"/>
-      <c r="B68" s="70"/>
+      <c r="A68" s="75"/>
+      <c r="B68" s="83"/>
       <c r="C68" s="3" t="s">
         <v>15</v>
       </c>
@@ -4883,23 +4899,23 @@
       <c r="E68" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="62" t="s">
+      <c r="F68" s="70" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="54"/>
-      <c r="B69" s="70"/>
-      <c r="C69" s="59" t="s">
+      <c r="A69" s="75"/>
+      <c r="B69" s="83"/>
+      <c r="C69" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D69" s="60"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="45"/>
+      <c r="D69" s="68"/>
+      <c r="E69" s="69"/>
+      <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="54"/>
-      <c r="B70" s="70"/>
+      <c r="A70" s="75"/>
+      <c r="B70" s="83"/>
       <c r="C70" s="1" t="s">
         <v>86</v>
       </c>
@@ -4909,21 +4925,21 @@
       <c r="E70" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F70" s="45"/>
+      <c r="F70" s="49"/>
     </row>
     <row r="71" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="54"/>
-      <c r="B71" s="70"/>
-      <c r="C71" s="59" t="s">
+      <c r="A71" s="75"/>
+      <c r="B71" s="83"/>
+      <c r="C71" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D71" s="60"/>
-      <c r="E71" s="61"/>
-      <c r="F71" s="45"/>
+      <c r="D71" s="68"/>
+      <c r="E71" s="69"/>
+      <c r="F71" s="49"/>
     </row>
     <row r="72" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="55"/>
-      <c r="B72" s="71"/>
+      <c r="A72" s="76"/>
+      <c r="B72" s="84"/>
       <c r="C72" s="1" t="s">
         <v>88</v>
       </c>
@@ -4933,27 +4949,27 @@
       <c r="E72" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F72" s="46"/>
+      <c r="F72" s="50"/>
     </row>
     <row r="73" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="53" t="s">
+      <c r="A73" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="B73" s="56" t="s">
+      <c r="B73" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="C73" s="59" t="s">
+      <c r="C73" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D73" s="60"/>
-      <c r="E73" s="61"/>
-      <c r="F73" s="62" t="s">
+      <c r="D73" s="68"/>
+      <c r="E73" s="69"/>
+      <c r="F73" s="70" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="54"/>
-      <c r="B74" s="57"/>
+      <c r="A74" s="75"/>
+      <c r="B74" s="72"/>
       <c r="C74" s="3" t="s">
         <v>22</v>
       </c>
@@ -4963,39 +4979,39 @@
       <c r="E74" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F74" s="45"/>
+      <c r="F74" s="49"/>
     </row>
     <row r="75" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="54"/>
-      <c r="B75" s="57"/>
-      <c r="C75" s="59" t="s">
+      <c r="A75" s="75"/>
+      <c r="B75" s="72"/>
+      <c r="C75" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D75" s="60"/>
-      <c r="E75" s="61"/>
-      <c r="F75" s="45"/>
+      <c r="D75" s="68"/>
+      <c r="E75" s="69"/>
+      <c r="F75" s="49"/>
     </row>
     <row r="76" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="54"/>
-      <c r="B76" s="57"/>
+      <c r="A76" s="75"/>
+      <c r="B76" s="72"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
-      <c r="F76" s="45"/>
+      <c r="F76" s="49"/>
     </row>
     <row r="77" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="54"/>
-      <c r="B77" s="57"/>
-      <c r="C77" s="59" t="s">
+      <c r="A77" s="75"/>
+      <c r="B77" s="72"/>
+      <c r="C77" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D77" s="60"/>
-      <c r="E77" s="61"/>
-      <c r="F77" s="45"/>
+      <c r="D77" s="68"/>
+      <c r="E77" s="69"/>
+      <c r="F77" s="49"/>
     </row>
     <row r="78" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="55"/>
-      <c r="B78" s="58"/>
+      <c r="A78" s="76"/>
+      <c r="B78" s="73"/>
       <c r="C78" s="1" t="s">
         <v>91</v>
       </c>
@@ -5005,25 +5021,25 @@
       <c r="E78" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F78" s="46"/>
+      <c r="F78" s="50"/>
     </row>
     <row r="79" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="53" t="s">
+      <c r="A79" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="B79" s="56" t="s">
+      <c r="B79" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="C79" s="59" t="s">
+      <c r="C79" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D79" s="60"/>
-      <c r="E79" s="61"/>
+      <c r="D79" s="68"/>
+      <c r="E79" s="69"/>
       <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="54"/>
-      <c r="B80" s="57"/>
+      <c r="A80" s="75"/>
+      <c r="B80" s="72"/>
       <c r="C80" s="3" t="s">
         <v>15</v>
       </c>
@@ -5033,23 +5049,23 @@
       <c r="E80" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F80" s="62" t="s">
+      <c r="F80" s="70" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="54"/>
-      <c r="B81" s="57"/>
-      <c r="C81" s="59" t="s">
+      <c r="A81" s="75"/>
+      <c r="B81" s="72"/>
+      <c r="C81" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D81" s="60"/>
-      <c r="E81" s="61"/>
-      <c r="F81" s="45"/>
+      <c r="D81" s="68"/>
+      <c r="E81" s="69"/>
+      <c r="F81" s="49"/>
     </row>
     <row r="82" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="54"/>
-      <c r="B82" s="57"/>
+      <c r="A82" s="75"/>
+      <c r="B82" s="72"/>
       <c r="C82" s="1" t="s">
         <v>94</v>
       </c>
@@ -5059,21 +5075,21 @@
       <c r="E82" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F82" s="45"/>
+      <c r="F82" s="49"/>
     </row>
     <row r="83" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="54"/>
-      <c r="B83" s="57"/>
-      <c r="C83" s="59" t="s">
+      <c r="A83" s="75"/>
+      <c r="B83" s="72"/>
+      <c r="C83" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D83" s="60"/>
-      <c r="E83" s="61"/>
-      <c r="F83" s="45"/>
+      <c r="D83" s="68"/>
+      <c r="E83" s="69"/>
+      <c r="F83" s="49"/>
     </row>
     <row r="84" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="55"/>
-      <c r="B84" s="58"/>
+      <c r="A84" s="76"/>
+      <c r="B84" s="73"/>
       <c r="C84" s="3" t="s">
         <v>96</v>
       </c>
@@ -5083,27 +5099,27 @@
       <c r="E84" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F84" s="46"/>
+      <c r="F84" s="50"/>
     </row>
     <row r="85" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="53" t="s">
+      <c r="A85" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="B85" s="56" t="s">
+      <c r="B85" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="C85" s="59" t="s">
+      <c r="C85" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D85" s="60"/>
-      <c r="E85" s="61"/>
-      <c r="F85" s="62" t="s">
+      <c r="D85" s="68"/>
+      <c r="E85" s="69"/>
+      <c r="F85" s="70" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="54"/>
-      <c r="B86" s="57"/>
+      <c r="A86" s="75"/>
+      <c r="B86" s="72"/>
       <c r="C86" s="3" t="s">
         <v>22</v>
       </c>
@@ -5113,39 +5129,39 @@
       <c r="E86" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F86" s="45"/>
+      <c r="F86" s="49"/>
     </row>
     <row r="87" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="54"/>
-      <c r="B87" s="57"/>
-      <c r="C87" s="59" t="s">
+      <c r="A87" s="75"/>
+      <c r="B87" s="72"/>
+      <c r="C87" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D87" s="60"/>
-      <c r="E87" s="61"/>
-      <c r="F87" s="45"/>
+      <c r="D87" s="68"/>
+      <c r="E87" s="69"/>
+      <c r="F87" s="49"/>
     </row>
     <row r="88" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="54"/>
-      <c r="B88" s="57"/>
+      <c r="A88" s="75"/>
+      <c r="B88" s="72"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
-      <c r="F88" s="45"/>
+      <c r="F88" s="49"/>
     </row>
     <row r="89" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="54"/>
-      <c r="B89" s="57"/>
-      <c r="C89" s="59" t="s">
+      <c r="A89" s="75"/>
+      <c r="B89" s="72"/>
+      <c r="C89" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D89" s="60"/>
-      <c r="E89" s="61"/>
-      <c r="F89" s="45"/>
+      <c r="D89" s="68"/>
+      <c r="E89" s="69"/>
+      <c r="F89" s="49"/>
     </row>
     <row r="90" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="55"/>
-      <c r="B90" s="58"/>
+      <c r="A90" s="76"/>
+      <c r="B90" s="73"/>
       <c r="C90" s="1" t="s">
         <v>99</v>
       </c>
@@ -5155,25 +5171,25 @@
       <c r="E90" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F90" s="46"/>
+      <c r="F90" s="50"/>
     </row>
     <row r="91" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="53" t="s">
+      <c r="A91" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B91" s="69" t="s">
+      <c r="B91" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="C91" s="59" t="s">
+      <c r="C91" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D91" s="60"/>
-      <c r="E91" s="61"/>
+      <c r="D91" s="68"/>
+      <c r="E91" s="69"/>
       <c r="F91" s="9"/>
     </row>
     <row r="92" spans="1:6" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="54"/>
-      <c r="B92" s="70"/>
+      <c r="A92" s="75"/>
+      <c r="B92" s="83"/>
       <c r="C92" s="3" t="s">
         <v>15</v>
       </c>
@@ -5183,23 +5199,23 @@
       <c r="E92" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F92" s="62" t="s">
+      <c r="F92" s="70" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="54"/>
-      <c r="B93" s="70"/>
-      <c r="C93" s="59" t="s">
+      <c r="A93" s="75"/>
+      <c r="B93" s="83"/>
+      <c r="C93" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D93" s="60"/>
-      <c r="E93" s="61"/>
-      <c r="F93" s="45"/>
+      <c r="D93" s="68"/>
+      <c r="E93" s="69"/>
+      <c r="F93" s="49"/>
     </row>
     <row r="94" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="54"/>
-      <c r="B94" s="70"/>
+      <c r="A94" s="75"/>
+      <c r="B94" s="83"/>
       <c r="C94" s="3" t="s">
         <v>103</v>
       </c>
@@ -5209,21 +5225,21 @@
       <c r="E94" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F94" s="45"/>
+      <c r="F94" s="49"/>
     </row>
     <row r="95" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="54"/>
-      <c r="B95" s="70"/>
-      <c r="C95" s="59" t="s">
+      <c r="A95" s="75"/>
+      <c r="B95" s="83"/>
+      <c r="C95" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D95" s="60"/>
-      <c r="E95" s="61"/>
-      <c r="F95" s="45"/>
+      <c r="D95" s="68"/>
+      <c r="E95" s="69"/>
+      <c r="F95" s="49"/>
     </row>
     <row r="96" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="55"/>
-      <c r="B96" s="71"/>
+      <c r="A96" s="76"/>
+      <c r="B96" s="84"/>
       <c r="C96" s="3" t="s">
         <v>105</v>
       </c>
@@ -5233,27 +5249,27 @@
       <c r="E96" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F96" s="46"/>
+      <c r="F96" s="50"/>
     </row>
     <row r="97" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="53" t="s">
+      <c r="A97" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B97" s="56" t="s">
+      <c r="B97" s="71" t="s">
         <v>106</v>
       </c>
-      <c r="C97" s="59" t="s">
+      <c r="C97" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D97" s="60"/>
-      <c r="E97" s="61"/>
-      <c r="F97" s="62" t="s">
+      <c r="D97" s="68"/>
+      <c r="E97" s="69"/>
+      <c r="F97" s="70" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="54"/>
-      <c r="B98" s="57"/>
+      <c r="A98" s="75"/>
+      <c r="B98" s="72"/>
       <c r="C98" s="3" t="s">
         <v>22</v>
       </c>
@@ -5263,39 +5279,39 @@
       <c r="E98" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F98" s="45"/>
+      <c r="F98" s="49"/>
     </row>
     <row r="99" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="54"/>
-      <c r="B99" s="57"/>
-      <c r="C99" s="59" t="s">
+      <c r="A99" s="75"/>
+      <c r="B99" s="72"/>
+      <c r="C99" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D99" s="60"/>
-      <c r="E99" s="61"/>
-      <c r="F99" s="45"/>
+      <c r="D99" s="68"/>
+      <c r="E99" s="69"/>
+      <c r="F99" s="49"/>
     </row>
     <row r="100" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="54"/>
-      <c r="B100" s="57"/>
+      <c r="A100" s="75"/>
+      <c r="B100" s="72"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
-      <c r="F100" s="45"/>
+      <c r="F100" s="49"/>
     </row>
     <row r="101" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="54"/>
-      <c r="B101" s="57"/>
-      <c r="C101" s="59" t="s">
+      <c r="A101" s="75"/>
+      <c r="B101" s="72"/>
+      <c r="C101" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D101" s="60"/>
-      <c r="E101" s="61"/>
-      <c r="F101" s="45"/>
+      <c r="D101" s="68"/>
+      <c r="E101" s="69"/>
+      <c r="F101" s="49"/>
     </row>
     <row r="102" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="55"/>
-      <c r="B102" s="58"/>
+      <c r="A102" s="76"/>
+      <c r="B102" s="73"/>
       <c r="C102" s="1" t="s">
         <v>108</v>
       </c>
@@ -5305,23 +5321,23 @@
       <c r="E102" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F102" s="46"/>
+      <c r="F102" s="50"/>
     </row>
     <row r="103" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="11"/>
       <c r="B103" s="11"/>
-      <c r="C103" s="59" t="s">
+      <c r="C103" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D103" s="60"/>
-      <c r="E103" s="61"/>
+      <c r="D103" s="68"/>
+      <c r="E103" s="69"/>
       <c r="F103" s="12"/>
     </row>
     <row r="104" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="54" t="s">
+      <c r="A104" s="75" t="s">
         <v>100</v>
       </c>
-      <c r="B104" s="57" t="s">
+      <c r="B104" s="72" t="s">
         <v>106</v>
       </c>
       <c r="C104" s="10" t="s">
@@ -5333,23 +5349,23 @@
       <c r="E104" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F104" s="62" t="s">
+      <c r="F104" s="70" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="54"/>
-      <c r="B105" s="57"/>
-      <c r="C105" s="59" t="s">
+      <c r="A105" s="75"/>
+      <c r="B105" s="72"/>
+      <c r="C105" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D105" s="60"/>
-      <c r="E105" s="61"/>
-      <c r="F105" s="45"/>
+      <c r="D105" s="68"/>
+      <c r="E105" s="69"/>
+      <c r="F105" s="49"/>
     </row>
     <row r="106" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="54"/>
-      <c r="B106" s="57"/>
+      <c r="A106" s="75"/>
+      <c r="B106" s="72"/>
       <c r="C106" s="1" t="s">
         <v>94</v>
       </c>
@@ -5359,21 +5375,21 @@
       <c r="E106" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F106" s="45"/>
+      <c r="F106" s="49"/>
     </row>
     <row r="107" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="54"/>
-      <c r="B107" s="57"/>
-      <c r="C107" s="59" t="s">
+      <c r="A107" s="75"/>
+      <c r="B107" s="72"/>
+      <c r="C107" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D107" s="60"/>
-      <c r="E107" s="61"/>
-      <c r="F107" s="45"/>
+      <c r="D107" s="68"/>
+      <c r="E107" s="69"/>
+      <c r="F107" s="49"/>
     </row>
     <row r="108" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="55"/>
-      <c r="B108" s="58"/>
+      <c r="A108" s="76"/>
+      <c r="B108" s="73"/>
       <c r="C108" s="3" t="s">
         <v>110</v>
       </c>
@@ -5383,27 +5399,27 @@
       <c r="E108" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F108" s="46"/>
+      <c r="F108" s="50"/>
     </row>
     <row r="109" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="53" t="s">
+      <c r="A109" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B109" s="56" t="s">
+      <c r="B109" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="C109" s="59" t="s">
+      <c r="C109" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D109" s="60"/>
-      <c r="E109" s="61"/>
-      <c r="F109" s="62" t="s">
+      <c r="D109" s="68"/>
+      <c r="E109" s="69"/>
+      <c r="F109" s="70" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="54"/>
-      <c r="B110" s="57"/>
+      <c r="A110" s="75"/>
+      <c r="B110" s="72"/>
       <c r="C110" s="3" t="s">
         <v>22</v>
       </c>
@@ -5413,39 +5429,39 @@
       <c r="E110" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F110" s="45"/>
+      <c r="F110" s="49"/>
     </row>
     <row r="111" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="54"/>
-      <c r="B111" s="57"/>
-      <c r="C111" s="59" t="s">
+      <c r="A111" s="75"/>
+      <c r="B111" s="72"/>
+      <c r="C111" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D111" s="60"/>
-      <c r="E111" s="61"/>
-      <c r="F111" s="45"/>
+      <c r="D111" s="68"/>
+      <c r="E111" s="69"/>
+      <c r="F111" s="49"/>
     </row>
     <row r="112" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="54"/>
-      <c r="B112" s="57"/>
+      <c r="A112" s="75"/>
+      <c r="B112" s="72"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
-      <c r="F112" s="45"/>
+      <c r="F112" s="49"/>
     </row>
     <row r="113" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="54"/>
-      <c r="B113" s="57"/>
-      <c r="C113" s="59" t="s">
+      <c r="A113" s="75"/>
+      <c r="B113" s="72"/>
+      <c r="C113" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D113" s="60"/>
-      <c r="E113" s="61"/>
-      <c r="F113" s="45"/>
+      <c r="D113" s="68"/>
+      <c r="E113" s="69"/>
+      <c r="F113" s="49"/>
     </row>
     <row r="114" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="55"/>
-      <c r="B114" s="58"/>
+      <c r="A114" s="76"/>
+      <c r="B114" s="73"/>
       <c r="C114" s="1" t="s">
         <v>113</v>
       </c>
@@ -5455,25 +5471,25 @@
       <c r="E114" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F114" s="46"/>
+      <c r="F114" s="50"/>
     </row>
     <row r="115" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="53" t="s">
+      <c r="A115" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B115" s="56" t="s">
+      <c r="B115" s="71" t="s">
         <v>114</v>
       </c>
-      <c r="C115" s="59" t="s">
+      <c r="C115" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D115" s="60"/>
-      <c r="E115" s="61"/>
+      <c r="D115" s="68"/>
+      <c r="E115" s="69"/>
       <c r="F115" s="9"/>
     </row>
     <row r="116" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="54"/>
-      <c r="B116" s="57"/>
+      <c r="A116" s="75"/>
+      <c r="B116" s="72"/>
       <c r="C116" s="3" t="s">
         <v>15</v>
       </c>
@@ -5483,23 +5499,23 @@
       <c r="E116" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F116" s="62" t="s">
+      <c r="F116" s="70" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="54"/>
-      <c r="B117" s="57"/>
-      <c r="C117" s="59" t="s">
+      <c r="A117" s="75"/>
+      <c r="B117" s="72"/>
+      <c r="C117" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D117" s="60"/>
-      <c r="E117" s="61"/>
-      <c r="F117" s="45"/>
+      <c r="D117" s="68"/>
+      <c r="E117" s="69"/>
+      <c r="F117" s="49"/>
     </row>
     <row r="118" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="54"/>
-      <c r="B118" s="57"/>
+      <c r="A118" s="75"/>
+      <c r="B118" s="72"/>
       <c r="C118" s="3" t="s">
         <v>60</v>
       </c>
@@ -5509,21 +5525,21 @@
       <c r="E118" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F118" s="45"/>
+      <c r="F118" s="49"/>
     </row>
     <row r="119" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="54"/>
-      <c r="B119" s="57"/>
-      <c r="C119" s="59" t="s">
+      <c r="A119" s="75"/>
+      <c r="B119" s="72"/>
+      <c r="C119" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D119" s="60"/>
-      <c r="E119" s="61"/>
-      <c r="F119" s="45"/>
+      <c r="D119" s="68"/>
+      <c r="E119" s="69"/>
+      <c r="F119" s="49"/>
     </row>
     <row r="120" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="55"/>
-      <c r="B120" s="58"/>
+      <c r="A120" s="76"/>
+      <c r="B120" s="73"/>
       <c r="C120" s="3" t="s">
         <v>116</v>
       </c>
@@ -5533,27 +5549,27 @@
       <c r="E120" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F120" s="46"/>
+      <c r="F120" s="50"/>
     </row>
     <row r="121" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="53" t="s">
+      <c r="A121" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B121" s="56" t="s">
+      <c r="B121" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="C121" s="59" t="s">
+      <c r="C121" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D121" s="60"/>
-      <c r="E121" s="61"/>
-      <c r="F121" s="62" t="s">
+      <c r="D121" s="68"/>
+      <c r="E121" s="69"/>
+      <c r="F121" s="70" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="54"/>
-      <c r="B122" s="57"/>
+      <c r="A122" s="75"/>
+      <c r="B122" s="72"/>
       <c r="C122" s="3" t="s">
         <v>22</v>
       </c>
@@ -5563,39 +5579,39 @@
       <c r="E122" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F122" s="45"/>
+      <c r="F122" s="49"/>
     </row>
     <row r="123" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="54"/>
-      <c r="B123" s="57"/>
-      <c r="C123" s="59" t="s">
+      <c r="A123" s="75"/>
+      <c r="B123" s="72"/>
+      <c r="C123" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D123" s="60"/>
-      <c r="E123" s="61"/>
-      <c r="F123" s="45"/>
+      <c r="D123" s="68"/>
+      <c r="E123" s="69"/>
+      <c r="F123" s="49"/>
     </row>
     <row r="124" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="54"/>
-      <c r="B124" s="57"/>
+      <c r="A124" s="75"/>
+      <c r="B124" s="72"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
-      <c r="F124" s="45"/>
+      <c r="F124" s="49"/>
     </row>
     <row r="125" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="54"/>
-      <c r="B125" s="57"/>
-      <c r="C125" s="59" t="s">
+      <c r="A125" s="75"/>
+      <c r="B125" s="72"/>
+      <c r="C125" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D125" s="60"/>
-      <c r="E125" s="61"/>
-      <c r="F125" s="45"/>
+      <c r="D125" s="68"/>
+      <c r="E125" s="69"/>
+      <c r="F125" s="49"/>
     </row>
     <row r="126" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="55"/>
-      <c r="B126" s="58"/>
+      <c r="A126" s="76"/>
+      <c r="B126" s="73"/>
       <c r="C126" s="1" t="s">
         <v>119</v>
       </c>
@@ -5605,25 +5621,25 @@
       <c r="E126" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F126" s="46"/>
+      <c r="F126" s="50"/>
     </row>
     <row r="127" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="53" t="s">
+      <c r="A127" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B127" s="56" t="s">
+      <c r="B127" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="C127" s="59" t="s">
+      <c r="C127" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D127" s="60"/>
-      <c r="E127" s="61"/>
+      <c r="D127" s="68"/>
+      <c r="E127" s="69"/>
       <c r="F127" s="9"/>
     </row>
     <row r="128" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="54"/>
-      <c r="B128" s="57"/>
+      <c r="A128" s="75"/>
+      <c r="B128" s="72"/>
       <c r="C128" s="3" t="s">
         <v>15</v>
       </c>
@@ -5633,23 +5649,23 @@
       <c r="E128" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F128" s="62" t="s">
+      <c r="F128" s="70" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="54"/>
-      <c r="B129" s="57"/>
-      <c r="C129" s="59" t="s">
+      <c r="A129" s="75"/>
+      <c r="B129" s="72"/>
+      <c r="C129" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D129" s="60"/>
-      <c r="E129" s="61"/>
-      <c r="F129" s="45"/>
+      <c r="D129" s="68"/>
+      <c r="E129" s="69"/>
+      <c r="F129" s="49"/>
     </row>
     <row r="130" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="54"/>
-      <c r="B130" s="57"/>
+      <c r="A130" s="75"/>
+      <c r="B130" s="72"/>
       <c r="C130" s="1" t="s">
         <v>122</v>
       </c>
@@ -5659,21 +5675,21 @@
       <c r="E130" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F130" s="45"/>
+      <c r="F130" s="49"/>
     </row>
     <row r="131" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="54"/>
-      <c r="B131" s="57"/>
-      <c r="C131" s="59" t="s">
+      <c r="A131" s="75"/>
+      <c r="B131" s="72"/>
+      <c r="C131" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D131" s="60"/>
-      <c r="E131" s="61"/>
-      <c r="F131" s="45"/>
+      <c r="D131" s="68"/>
+      <c r="E131" s="69"/>
+      <c r="F131" s="49"/>
     </row>
     <row r="132" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="55"/>
-      <c r="B132" s="58"/>
+      <c r="A132" s="76"/>
+      <c r="B132" s="73"/>
       <c r="C132" s="1" t="s">
         <v>124</v>
       </c>
@@ -5683,27 +5699,27 @@
       <c r="E132" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F132" s="46"/>
+      <c r="F132" s="50"/>
     </row>
     <row r="133" spans="1:6" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="53" t="s">
+      <c r="A133" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B133" s="56" t="s">
+      <c r="B133" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="C133" s="59" t="s">
+      <c r="C133" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D133" s="60"/>
-      <c r="E133" s="61"/>
-      <c r="F133" s="62" t="s">
+      <c r="D133" s="68"/>
+      <c r="E133" s="69"/>
+      <c r="F133" s="70" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="54"/>
-      <c r="B134" s="57"/>
+      <c r="A134" s="75"/>
+      <c r="B134" s="72"/>
       <c r="C134" s="3" t="s">
         <v>22</v>
       </c>
@@ -5713,39 +5729,39 @@
       <c r="E134" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F134" s="45"/>
+      <c r="F134" s="49"/>
     </row>
     <row r="135" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="54"/>
-      <c r="B135" s="57"/>
-      <c r="C135" s="59" t="s">
+      <c r="A135" s="75"/>
+      <c r="B135" s="72"/>
+      <c r="C135" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D135" s="60"/>
-      <c r="E135" s="61"/>
-      <c r="F135" s="45"/>
+      <c r="D135" s="68"/>
+      <c r="E135" s="69"/>
+      <c r="F135" s="49"/>
     </row>
     <row r="136" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="54"/>
-      <c r="B136" s="57"/>
+      <c r="A136" s="75"/>
+      <c r="B136" s="72"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
       <c r="E136" s="8"/>
-      <c r="F136" s="45"/>
+      <c r="F136" s="49"/>
     </row>
     <row r="137" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="54"/>
-      <c r="B137" s="57"/>
-      <c r="C137" s="59" t="s">
+      <c r="A137" s="75"/>
+      <c r="B137" s="72"/>
+      <c r="C137" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D137" s="60"/>
-      <c r="E137" s="61"/>
-      <c r="F137" s="45"/>
+      <c r="D137" s="68"/>
+      <c r="E137" s="69"/>
+      <c r="F137" s="49"/>
     </row>
     <row r="138" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="55"/>
-      <c r="B138" s="58"/>
+      <c r="A138" s="76"/>
+      <c r="B138" s="73"/>
       <c r="C138" s="3" t="s">
         <v>127</v>
       </c>
@@ -5755,25 +5771,25 @@
       <c r="E138" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F138" s="46"/>
+      <c r="F138" s="50"/>
     </row>
     <row r="139" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="63" t="s">
+      <c r="A139" s="77" t="s">
         <v>128</v>
       </c>
-      <c r="B139" s="66" t="s">
+      <c r="B139" s="80" t="s">
         <v>129</v>
       </c>
-      <c r="C139" s="59" t="s">
+      <c r="C139" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="D139" s="60"/>
-      <c r="E139" s="61"/>
+      <c r="D139" s="68"/>
+      <c r="E139" s="69"/>
       <c r="F139" s="9"/>
     </row>
     <row r="140" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="64"/>
-      <c r="B140" s="67"/>
+      <c r="A140" s="78"/>
+      <c r="B140" s="81"/>
       <c r="C140" s="3" t="s">
         <v>130</v>
       </c>
@@ -5783,23 +5799,23 @@
       <c r="E140" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F140" s="62" t="s">
+      <c r="F140" s="70" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="64"/>
-      <c r="B141" s="67"/>
-      <c r="C141" s="59" t="s">
+      <c r="A141" s="78"/>
+      <c r="B141" s="81"/>
+      <c r="C141" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D141" s="60"/>
-      <c r="E141" s="61"/>
-      <c r="F141" s="45"/>
+      <c r="D141" s="68"/>
+      <c r="E141" s="69"/>
+      <c r="F141" s="49"/>
     </row>
     <row r="142" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="64"/>
-      <c r="B142" s="67"/>
+      <c r="A142" s="78"/>
+      <c r="B142" s="81"/>
       <c r="C142" s="1" t="s">
         <v>132</v>
       </c>
@@ -5809,21 +5825,21 @@
       <c r="E142" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F142" s="45"/>
+      <c r="F142" s="49"/>
     </row>
     <row r="143" spans="1:6" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="64"/>
-      <c r="B143" s="67"/>
-      <c r="C143" s="59" t="s">
+      <c r="A143" s="78"/>
+      <c r="B143" s="81"/>
+      <c r="C143" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D143" s="60"/>
-      <c r="E143" s="61"/>
-      <c r="F143" s="45"/>
+      <c r="D143" s="68"/>
+      <c r="E143" s="69"/>
+      <c r="F143" s="49"/>
     </row>
     <row r="144" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="65"/>
-      <c r="B144" s="68"/>
+      <c r="A144" s="79"/>
+      <c r="B144" s="82"/>
       <c r="C144" s="3" t="s">
         <v>134</v>
       </c>
@@ -5833,10 +5849,142 @@
       <c r="E144" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F144" s="46"/>
+      <c r="F144" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="144">
+    <mergeCell ref="A133:A138"/>
+    <mergeCell ref="B133:B138"/>
+    <mergeCell ref="C133:E133"/>
+    <mergeCell ref="F133:F138"/>
+    <mergeCell ref="C135:E135"/>
+    <mergeCell ref="C137:E137"/>
+    <mergeCell ref="A139:A144"/>
+    <mergeCell ref="B139:B144"/>
+    <mergeCell ref="C139:E139"/>
+    <mergeCell ref="F140:F144"/>
+    <mergeCell ref="C141:E141"/>
+    <mergeCell ref="C143:E143"/>
+    <mergeCell ref="A121:A126"/>
+    <mergeCell ref="B121:B126"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="F121:F126"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="A127:A132"/>
+    <mergeCell ref="B127:B132"/>
+    <mergeCell ref="C127:E127"/>
+    <mergeCell ref="F128:F132"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="C131:E131"/>
+    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="B109:B114"/>
+    <mergeCell ref="C109:E109"/>
+    <mergeCell ref="F109:F114"/>
+    <mergeCell ref="C111:E111"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="B115:B120"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="F116:F120"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C119:E119"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="B97:B102"/>
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="F97:F102"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="B104:B108"/>
+    <mergeCell ref="F104:F108"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="C107:E107"/>
+    <mergeCell ref="A85:A90"/>
+    <mergeCell ref="B85:B90"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="F85:F90"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="B91:B96"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="F92:F96"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C95:E95"/>
+    <mergeCell ref="A73:A78"/>
+    <mergeCell ref="B73:B78"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="F73:F78"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="A79:A84"/>
+    <mergeCell ref="B79:B84"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="F80:F84"/>
+    <mergeCell ref="C81:E81"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="A61:A66"/>
+    <mergeCell ref="B61:B66"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:F66"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="A67:A72"/>
+    <mergeCell ref="B67:B72"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="F68:F72"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="F49:F54"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="F56:F60"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="B43:B48"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="F44:F48"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:F30"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="A31:A36"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="B13:B18"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:F18"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C23:E23"/>
     <mergeCell ref="A1:A6"/>
     <mergeCell ref="B1:B6"/>
     <mergeCell ref="C1:E1"/>
@@ -5849,138 +5997,6 @@
     <mergeCell ref="F8:F12"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C11:E11"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:F18"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:F30"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="A31:A36"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F32:F36"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="B43:B48"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F44:F48"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="F49:F54"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="F56:F60"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="A61:A66"/>
-    <mergeCell ref="B61:B66"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="F61:F66"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="A67:A72"/>
-    <mergeCell ref="B67:B72"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="F68:F72"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="A73:A78"/>
-    <mergeCell ref="B73:B78"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="F73:F78"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="A79:A84"/>
-    <mergeCell ref="B79:B84"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="F80:F84"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="A85:A90"/>
-    <mergeCell ref="B85:B90"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="F85:F90"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="B91:B96"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="F92:F96"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C95:E95"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="B97:B102"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="F97:F102"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="C101:E101"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="B104:B108"/>
-    <mergeCell ref="F104:F108"/>
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="C107:E107"/>
-    <mergeCell ref="A109:A114"/>
-    <mergeCell ref="B109:B114"/>
-    <mergeCell ref="C109:E109"/>
-    <mergeCell ref="F109:F114"/>
-    <mergeCell ref="C111:E111"/>
-    <mergeCell ref="C113:E113"/>
-    <mergeCell ref="A115:A120"/>
-    <mergeCell ref="B115:B120"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="F116:F120"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="C119:E119"/>
-    <mergeCell ref="A121:A126"/>
-    <mergeCell ref="B121:B126"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="F121:F126"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C125:E125"/>
-    <mergeCell ref="A127:A132"/>
-    <mergeCell ref="B127:B132"/>
-    <mergeCell ref="C127:E127"/>
-    <mergeCell ref="F128:F132"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="C131:E131"/>
-    <mergeCell ref="A133:A138"/>
-    <mergeCell ref="B133:B138"/>
-    <mergeCell ref="C133:E133"/>
-    <mergeCell ref="F133:F138"/>
-    <mergeCell ref="C135:E135"/>
-    <mergeCell ref="C137:E137"/>
-    <mergeCell ref="A139:A144"/>
-    <mergeCell ref="B139:B144"/>
-    <mergeCell ref="C139:E139"/>
-    <mergeCell ref="F140:F144"/>
-    <mergeCell ref="C141:E141"/>
-    <mergeCell ref="C143:E143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6005,35 +6021,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="86" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="98"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="88"/>
     </row>
     <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="56"/>
-      <c r="B2" s="99" t="s">
+      <c r="A2" s="71"/>
+      <c r="B2" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="99" t="s">
+      <c r="C2" s="89" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="101" t="s">
+      <c r="D2" s="91" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="102"/>
+      <c r="E2" s="92"/>
       <c r="F2" s="1" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="58"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
+      <c r="A3" s="73"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
       <c r="D3" s="15" t="s">
         <v>140</v>
       </c>
@@ -6045,7 +6061,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="93" t="s">
         <v>142</v>
       </c>
       <c r="B4" s="16">
@@ -6063,7 +6079,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="27.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="79"/>
+      <c r="A5" s="94"/>
       <c r="B5" s="16">
         <v>2</v>
       </c>
@@ -6079,7 +6095,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="79"/>
+      <c r="A6" s="94"/>
       <c r="B6" s="16">
         <v>3</v>
       </c>
@@ -6089,7 +6105,7 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="80"/>
+      <c r="A7" s="95"/>
       <c r="B7" s="16">
         <v>4</v>
       </c>
@@ -6099,7 +6115,7 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="96" t="s">
         <v>146</v>
       </c>
       <c r="B8" s="16">
@@ -6117,7 +6133,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="82"/>
+      <c r="A9" s="97"/>
       <c r="B9" s="16">
         <v>2</v>
       </c>
@@ -6133,7 +6149,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="82"/>
+      <c r="A10" s="97"/>
       <c r="B10" s="16">
         <v>3</v>
       </c>
@@ -6143,7 +6159,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="83"/>
+      <c r="A11" s="98"/>
       <c r="B11" s="16">
         <v>4</v>
       </c>
@@ -6157,66 +6173,61 @@
       <c r="B12" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="99" t="s">
         <v>150</v>
       </c>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="86"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="101"/>
     </row>
     <row r="13" spans="1:6" ht="22.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="96" t="s">
         <v>151</v>
       </c>
       <c r="B13" s="16">
         <v>1</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="C13" s="102" t="s">
         <v>152</v>
       </c>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="89"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="104"/>
     </row>
     <row r="14" spans="1:6" ht="22.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="82"/>
+      <c r="A14" s="97"/>
       <c r="B14" s="16">
         <v>2</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="102" t="s">
         <v>153</v>
       </c>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="89"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="104"/>
     </row>
     <row r="15" spans="1:6" ht="22.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="82"/>
+      <c r="A15" s="97"/>
       <c r="B15" s="16">
         <v>3</v>
       </c>
-      <c r="C15" s="90"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="92"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="107"/>
     </row>
     <row r="16" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="82"/>
+      <c r="A16" s="97"/>
       <c r="B16" s="16">
         <v>4</v>
       </c>
-      <c r="C16" s="93"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="95"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="109"/>
+      <c r="F16" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="C12:F12"/>
@@ -6225,6 +6236,11 @@
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F16"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:E2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C13" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -6251,12 +6267,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="99" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="86"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="101"/>
     </row>
     <row r="2" spans="1:6" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -6288,7 +6304,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="111" t="s">
         <v>162</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -6298,7 +6314,7 @@
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="104"/>
+      <c r="A5" s="112"/>
       <c r="B5" s="8" t="s">
         <v>164</v>
       </c>

</xml_diff>